<commit_message>
updated some view information
</commit_message>
<xml_diff>
--- a/Research_Bucket/Android_UserRatings/data/Spring_2015/Spring2015.xlsx
+++ b/Research_Bucket/Android_UserRatings/data/Spring_2015/Spring2015.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="155">
   <si>
     <t>Genre</t>
   </si>
@@ -297,6 +297,189 @@
   </si>
   <si>
     <t>ZTE WiFi Monitor</t>
+  </si>
+  <si>
+    <t>ESPN 950 WXGI</t>
+  </si>
+  <si>
+    <t>짝지 - 짝사랑 매칭</t>
+  </si>
+  <si>
+    <t>PakistanCall 완전 무료 파키스탄 전화</t>
+  </si>
+  <si>
+    <t>女性生理期瘦身小秘書</t>
+  </si>
+  <si>
+    <t>AutoSMS</t>
+  </si>
+  <si>
+    <t>방송통신위원회</t>
+  </si>
+  <si>
+    <t>Parental Control for Mobile</t>
+  </si>
+  <si>
+    <t>86무료국제전화</t>
+  </si>
+  <si>
+    <t>HarbourCity Guide</t>
+  </si>
+  <si>
+    <t>FTSE</t>
+  </si>
+  <si>
+    <t>12合1實用工具箱(480*800)</t>
+  </si>
+  <si>
+    <t>Gandul.info</t>
+  </si>
+  <si>
+    <t>Philip F.- Tennis Betting Tips</t>
+  </si>
+  <si>
+    <t>Connect to S800c</t>
+  </si>
+  <si>
+    <t>World of Goo Guide</t>
+  </si>
+  <si>
+    <t>Fan Angry Birds</t>
+  </si>
+  <si>
+    <t>Wellness</t>
+  </si>
+  <si>
+    <t>FaxDocument Send Fax Instantly</t>
+  </si>
+  <si>
+    <t>Easy Recall</t>
+  </si>
+  <si>
+    <t>Daily Bible Verse</t>
+  </si>
+  <si>
+    <t>Fiches Révisions Bac S, ES, L</t>
+  </si>
+  <si>
+    <t>Racing Boats</t>
+  </si>
+  <si>
+    <t>翼支付</t>
+  </si>
+  <si>
+    <t>ギャラリーマップ</t>
+  </si>
+  <si>
+    <t>Real Ghost Finder Lite</t>
+  </si>
+  <si>
+    <t>Photo Partner Match</t>
+  </si>
+  <si>
+    <t>EasyN</t>
+  </si>
+  <si>
+    <t>Palumbo Sila Webcam</t>
+  </si>
+  <si>
+    <t>So-netブログ</t>
+  </si>
+  <si>
+    <t>Mileage Tracker</t>
+  </si>
+  <si>
+    <t>3D Urban Madness</t>
+  </si>
+  <si>
+    <t>Racing</t>
+  </si>
+  <si>
+    <t>Smart Task Manager FREE</t>
+  </si>
+  <si>
+    <t>SpyPhone by MAGMA</t>
+  </si>
+  <si>
+    <t>FoxFi (WiFi Tether w/o Root)</t>
+  </si>
+  <si>
+    <t>Calculator Area &amp; Perimeter</t>
+  </si>
+  <si>
+    <t>(Lite)Memory Card (단어 암기 카드)</t>
+  </si>
+  <si>
+    <t>Call log Smart Extras™</t>
+  </si>
+  <si>
+    <t>Sportsgym Scandinavia</t>
+  </si>
+  <si>
+    <t>K-POP★Beat the Music ★Plus</t>
+  </si>
+  <si>
+    <t>Of Mice and Men</t>
+  </si>
+  <si>
+    <t>JALライブ壁紙　スケジュール版</t>
+  </si>
+  <si>
+    <t>WiFi Location Toggle</t>
+  </si>
+  <si>
+    <t>iSpeak</t>
+  </si>
+  <si>
+    <t>Kids University Lite</t>
+  </si>
+  <si>
+    <t>Decision Helper Free</t>
+  </si>
+  <si>
+    <t>Moon black &amp; white</t>
+  </si>
+  <si>
+    <t>Christmas songs free</t>
+  </si>
+  <si>
+    <t>3x battery saver - iBattery</t>
+  </si>
+  <si>
+    <t>mWydatki - mBank</t>
+  </si>
+  <si>
+    <t>Crossbow Shooting</t>
+  </si>
+  <si>
+    <t>페이씽크(ST-500용) 올밴</t>
+  </si>
+  <si>
+    <t>Army Rifle Marksmanship Guide</t>
+  </si>
+  <si>
+    <t>Smart Clipboard</t>
+  </si>
+  <si>
+    <t>Andaal Thiruppavai Pasurams</t>
+  </si>
+  <si>
+    <t>telview mobile cctv</t>
+  </si>
+  <si>
+    <t>Manner Camera</t>
+  </si>
+  <si>
+    <t>Star Wars Flashlight 911 Free</t>
+  </si>
+  <si>
+    <t>ViVirus</t>
+  </si>
+  <si>
+    <t>Islam - Salafi Manhaj - Dawah</t>
+  </si>
+  <si>
+    <t>Unit Converter</t>
   </si>
 </sst>
 </file>
@@ -2937,20 +3120,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O23"/>
+  <dimension ref="A1:Q53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="25.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2966,8 +3149,9 @@
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>45</v>
       </c>
@@ -2979,16 +3163,17 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="7"/>
+      <c r="K2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="K2" s="7"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
       <c r="N2" s="7"/>
       <c r="O2" s="7"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="7"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>57</v>
       </c>
@@ -3010,30 +3195,36 @@
       <c r="G3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="10" t="s">
+      <c r="H3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" s="3"/>
+      <c r="J3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="O3" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q3" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -3055,29 +3246,35 @@
       <c r="G4">
         <v>21.2</v>
       </c>
-      <c r="I4" t="s">
+      <c r="H4">
+        <v>51.11</v>
+      </c>
+      <c r="J4" t="s">
         <v>47</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>5</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>77</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <v>7658</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <v>6</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>77.92</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <v>7.8</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -3099,29 +3296,35 @@
       <c r="G5">
         <v>11</v>
       </c>
-      <c r="I5" t="s">
+      <c r="H5">
+        <v>51.25</v>
+      </c>
+      <c r="J5" t="s">
         <v>48</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>13</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>47</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <v>6605</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <v>3</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>63.83</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>63</v>
       </c>
@@ -3143,29 +3346,35 @@
       <c r="G6">
         <v>12</v>
       </c>
-      <c r="I6" t="s">
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
         <v>49</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>17</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>104</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>16524</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <v>6</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <v>57.69</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -3187,29 +3396,35 @@
       <c r="G7">
         <v>8.4</v>
       </c>
-      <c r="I7" t="s">
+      <c r="H7">
         <v>50</v>
       </c>
       <c r="J7" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" t="s">
         <v>13</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>54</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>5548</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <v>3</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>55.56</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -3231,29 +3446,35 @@
       <c r="G8">
         <v>6.6</v>
       </c>
-      <c r="I8" t="s">
+      <c r="H8">
+        <v>50</v>
+      </c>
+      <c r="J8" t="s">
         <v>51</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>33</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <v>55</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <v>5027</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <v>3</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>54.55</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -3275,29 +3496,35 @@
       <c r="G9">
         <v>5.6</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="J9" t="s">
         <v>52</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>10</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <v>94</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <v>9321</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <v>4</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <v>42.55</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -3319,29 +3546,35 @@
       <c r="G10">
         <v>6.3</v>
       </c>
-      <c r="I10" t="s">
-        <v>53</v>
+      <c r="H10">
+        <v>50</v>
       </c>
       <c r="J10" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" t="s">
         <v>5</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <v>118</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>13053</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <v>5</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>42.37</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -3363,29 +3596,35 @@
       <c r="G11">
         <v>4.3</v>
       </c>
-      <c r="I11" t="s">
-        <v>54</v>
+      <c r="H11">
+        <v>50</v>
       </c>
       <c r="J11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" t="s">
         <v>5</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <v>118</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>13053</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <v>5</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>42.37</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -3407,29 +3646,35 @@
       <c r="G12">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I12" t="s">
+      <c r="H12">
+        <v>51.11</v>
+      </c>
+      <c r="J12" t="s">
         <v>55</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>10</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>49</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>6829</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <v>2</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>40.82</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -3451,29 +3696,35 @@
       <c r="G13">
         <v>3.9</v>
       </c>
-      <c r="I13" t="s">
+      <c r="H13">
+        <v>51.11</v>
+      </c>
+      <c r="J13" t="s">
         <v>56</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>22</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <v>76</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <v>5648</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <v>3</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <v>39.47</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -3495,29 +3746,35 @@
       <c r="G14">
         <v>6.1</v>
       </c>
-      <c r="I14" t="s">
+      <c r="H14">
+        <v>52.63</v>
+      </c>
+      <c r="J14" t="s">
         <v>72</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>10</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>63</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>6333</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <v>2</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>31.75</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -3539,29 +3796,35 @@
       <c r="G15">
         <v>2.5</v>
       </c>
-      <c r="I15" t="s">
+      <c r="H15">
+        <v>50</v>
+      </c>
+      <c r="J15" t="s">
         <v>73</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>22</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>101</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <v>9474</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <v>3</v>
       </c>
-      <c r="N15">
+      <c r="O15">
         <v>29.7</v>
       </c>
-      <c r="O15">
+      <c r="P15">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>86</v>
       </c>
@@ -3583,29 +3846,35 @@
       <c r="G16">
         <v>2.5</v>
       </c>
-      <c r="I16" t="s">
+      <c r="H16">
+        <v>50</v>
+      </c>
+      <c r="J16" t="s">
         <v>74</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>33</v>
       </c>
-      <c r="K16">
+      <c r="L16">
         <v>202</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <v>22048</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <v>6</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>29.7</v>
       </c>
-      <c r="O16">
+      <c r="P16">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>87</v>
       </c>
@@ -3627,29 +3896,35 @@
       <c r="G17">
         <v>2.5</v>
       </c>
-      <c r="I17" t="s">
-        <v>75</v>
+      <c r="H17">
+        <v>50</v>
       </c>
       <c r="J17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K17">
-        <v>222</v>
+        <v>76</v>
+      </c>
+      <c r="K17" t="s">
+        <v>29</v>
       </c>
       <c r="L17">
-        <v>17354</v>
+        <v>74</v>
       </c>
       <c r="M17">
-        <v>6</v>
+        <v>8859</v>
       </c>
       <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
         <v>27.03</v>
       </c>
-      <c r="O17">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q17">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>88</v>
       </c>
@@ -3671,29 +3946,35 @@
       <c r="G18">
         <v>1.3</v>
       </c>
-      <c r="I18" t="s">
-        <v>76</v>
+      <c r="H18">
+        <v>50</v>
       </c>
       <c r="J18" t="s">
-        <v>29</v>
-      </c>
-      <c r="K18">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="K18" t="s">
+        <v>5</v>
       </c>
       <c r="L18">
-        <v>8859</v>
+        <v>222</v>
       </c>
       <c r="M18">
-        <v>2</v>
+        <v>17354</v>
       </c>
       <c r="N18">
+        <v>6</v>
+      </c>
+      <c r="O18">
         <v>27.03</v>
       </c>
-      <c r="O18">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <v>3.5</v>
+      </c>
+      <c r="Q18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -3715,29 +3996,35 @@
       <c r="G19">
         <v>4.3</v>
       </c>
-      <c r="I19" t="s">
-        <v>77</v>
+      <c r="H19">
+        <v>51.11</v>
       </c>
       <c r="J19" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19">
+        <v>78</v>
+      </c>
+      <c r="K19" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19">
         <v>156</v>
       </c>
-      <c r="L19">
-        <v>16342</v>
-      </c>
       <c r="M19">
+        <v>18119</v>
+      </c>
+      <c r="N19">
         <v>4</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <v>25.64</v>
       </c>
-      <c r="O19">
-        <v>2.4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P19">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -3759,29 +4046,35 @@
       <c r="G20">
         <v>3.2</v>
       </c>
-      <c r="I20" t="s">
-        <v>78</v>
+      <c r="H20">
+        <v>51.11</v>
       </c>
       <c r="J20" t="s">
-        <v>5</v>
-      </c>
-      <c r="K20">
+        <v>77</v>
+      </c>
+      <c r="K20" t="s">
+        <v>11</v>
+      </c>
+      <c r="L20">
         <v>156</v>
       </c>
-      <c r="L20">
-        <v>18119</v>
-      </c>
       <c r="M20">
+        <v>16342</v>
+      </c>
+      <c r="N20">
         <v>4</v>
       </c>
-      <c r="N20">
+      <c r="O20">
         <v>25.64</v>
       </c>
-      <c r="O20">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>2.4</v>
+      </c>
+      <c r="Q20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -3803,29 +4096,35 @@
       <c r="G21">
         <v>2.2000000000000002</v>
       </c>
-      <c r="I21" t="s">
+      <c r="H21">
+        <v>50</v>
+      </c>
+      <c r="J21" t="s">
         <v>79</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>33</v>
       </c>
-      <c r="K21">
+      <c r="L21">
         <v>82</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>5953</v>
       </c>
-      <c r="M21">
+      <c r="N21">
         <v>2</v>
       </c>
-      <c r="N21">
+      <c r="O21">
         <v>24.39</v>
       </c>
-      <c r="O21">
+      <c r="P21">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -3847,29 +4146,35 @@
       <c r="G22">
         <v>3</v>
       </c>
-      <c r="I22" t="s">
+      <c r="H22">
+        <v>50</v>
+      </c>
+      <c r="J22" t="s">
         <v>80</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>33</v>
       </c>
-      <c r="K22">
+      <c r="L22">
         <v>47</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>5987</v>
       </c>
-      <c r="M22">
+      <c r="N22">
         <v>1</v>
       </c>
-      <c r="N22">
+      <c r="O22">
         <v>21.28</v>
       </c>
-      <c r="O22">
+      <c r="P22">
         <v>1.7</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -3891,26 +4196,1532 @@
       <c r="G23">
         <v>3.1</v>
       </c>
-      <c r="I23" t="s">
+      <c r="H23">
+        <v>50</v>
+      </c>
+      <c r="J23" t="s">
         <v>81</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>10</v>
       </c>
-      <c r="K23">
+      <c r="L23">
         <v>1639</v>
       </c>
-      <c r="L23">
+      <c r="M23">
         <v>101057</v>
       </c>
-      <c r="M23">
+      <c r="N23">
         <v>34</v>
       </c>
-      <c r="N23">
+      <c r="O23">
         <v>20.74</v>
       </c>
-      <c r="O23">
+      <c r="P23">
         <v>3.4</v>
+      </c>
+      <c r="Q23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <v>90</v>
+      </c>
+      <c r="D24">
+        <v>11251</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <v>33.33</v>
+      </c>
+      <c r="G24">
+        <v>2.7</v>
+      </c>
+      <c r="H24">
+        <v>50</v>
+      </c>
+      <c r="J24" t="s">
+        <v>124</v>
+      </c>
+      <c r="K24" t="s">
+        <v>125</v>
+      </c>
+      <c r="L24">
+        <v>195</v>
+      </c>
+      <c r="M24">
+        <v>14565</v>
+      </c>
+      <c r="N24">
+        <v>4</v>
+      </c>
+      <c r="O24">
+        <v>20.51</v>
+      </c>
+      <c r="P24">
+        <v>2.7</v>
+      </c>
+      <c r="Q24">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>245</v>
+      </c>
+      <c r="D25">
+        <v>13027</v>
+      </c>
+      <c r="E25">
+        <v>8</v>
+      </c>
+      <c r="F25">
+        <v>32.65</v>
+      </c>
+      <c r="G25">
+        <v>6.1</v>
+      </c>
+      <c r="H25">
+        <v>50</v>
+      </c>
+      <c r="J25" t="s">
+        <v>126</v>
+      </c>
+      <c r="K25" t="s">
+        <v>33</v>
+      </c>
+      <c r="L25">
+        <v>51</v>
+      </c>
+      <c r="M25">
+        <v>7742</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>19.61</v>
+      </c>
+      <c r="P25">
+        <v>1.3</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26">
+        <v>97</v>
+      </c>
+      <c r="D26">
+        <v>7443</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>30.93</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>50</v>
+      </c>
+      <c r="J26" t="s">
+        <v>127</v>
+      </c>
+      <c r="K26" t="s">
+        <v>33</v>
+      </c>
+      <c r="L26">
+        <v>468</v>
+      </c>
+      <c r="M26">
+        <v>63529</v>
+      </c>
+      <c r="N26">
+        <v>9</v>
+      </c>
+      <c r="O26">
+        <v>19.23</v>
+      </c>
+      <c r="P26">
+        <v>1.4</v>
+      </c>
+      <c r="Q26">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27">
+        <v>67</v>
+      </c>
+      <c r="D27">
+        <v>7887</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>29.85</v>
+      </c>
+      <c r="G27">
+        <v>2.5</v>
+      </c>
+      <c r="H27">
+        <v>50</v>
+      </c>
+      <c r="J27" t="s">
+        <v>128</v>
+      </c>
+      <c r="K27" t="s">
+        <v>10</v>
+      </c>
+      <c r="L27">
+        <v>113</v>
+      </c>
+      <c r="M27">
+        <v>11323</v>
+      </c>
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>17.7</v>
+      </c>
+      <c r="P27">
+        <v>1.8</v>
+      </c>
+      <c r="Q27">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <v>68</v>
+      </c>
+      <c r="D28">
+        <v>7938</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>29.41</v>
+      </c>
+      <c r="G28">
+        <v>2.5</v>
+      </c>
+      <c r="H28">
+        <v>50</v>
+      </c>
+      <c r="J28" t="s">
+        <v>129</v>
+      </c>
+      <c r="K28" t="s">
+        <v>33</v>
+      </c>
+      <c r="L28">
+        <v>115</v>
+      </c>
+      <c r="M28">
+        <v>11089</v>
+      </c>
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>17.39</v>
+      </c>
+      <c r="P28">
+        <v>1.8</v>
+      </c>
+      <c r="Q28">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>146</v>
+      </c>
+      <c r="D29">
+        <v>10707</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29">
+        <v>27.4</v>
+      </c>
+      <c r="G29">
+        <v>3.7</v>
+      </c>
+      <c r="H29">
+        <v>50</v>
+      </c>
+      <c r="J29" t="s">
+        <v>130</v>
+      </c>
+      <c r="K29" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29">
+        <v>118</v>
+      </c>
+      <c r="M29">
+        <v>9919</v>
+      </c>
+      <c r="N29">
+        <v>2</v>
+      </c>
+      <c r="O29">
+        <v>16.95</v>
+      </c>
+      <c r="P29">
+        <v>2</v>
+      </c>
+      <c r="Q29">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>113</v>
+      </c>
+      <c r="D30">
+        <v>8926</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+      <c r="F30">
+        <v>26.55</v>
+      </c>
+      <c r="G30">
+        <v>3.4</v>
+      </c>
+      <c r="H30">
+        <v>50</v>
+      </c>
+      <c r="J30" t="s">
+        <v>131</v>
+      </c>
+      <c r="K30" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30">
+        <v>124</v>
+      </c>
+      <c r="M30">
+        <v>7872</v>
+      </c>
+      <c r="N30">
+        <v>2</v>
+      </c>
+      <c r="O30">
+        <v>16.13</v>
+      </c>
+      <c r="P30">
+        <v>2.5</v>
+      </c>
+      <c r="Q30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31">
+        <v>193</v>
+      </c>
+      <c r="D31">
+        <v>14202</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>25.91</v>
+      </c>
+      <c r="G31">
+        <v>3.5</v>
+      </c>
+      <c r="H31">
+        <v>50</v>
+      </c>
+      <c r="J31" t="s">
+        <v>132</v>
+      </c>
+      <c r="K31" t="s">
+        <v>15</v>
+      </c>
+      <c r="L31">
+        <v>125</v>
+      </c>
+      <c r="M31">
+        <v>8670</v>
+      </c>
+      <c r="N31">
+        <v>2</v>
+      </c>
+      <c r="O31">
+        <v>16</v>
+      </c>
+      <c r="P31">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q31">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32">
+        <v>79</v>
+      </c>
+      <c r="D32">
+        <v>8874</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>25.32</v>
+      </c>
+      <c r="G32">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H32">
+        <v>50</v>
+      </c>
+      <c r="J32" t="s">
+        <v>133</v>
+      </c>
+      <c r="K32" t="s">
+        <v>3</v>
+      </c>
+      <c r="L32">
+        <v>321</v>
+      </c>
+      <c r="M32">
+        <v>30825</v>
+      </c>
+      <c r="N32">
+        <v>5</v>
+      </c>
+      <c r="O32">
+        <v>15.58</v>
+      </c>
+      <c r="P32">
+        <v>1.6</v>
+      </c>
+      <c r="Q32">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>81</v>
+      </c>
+      <c r="D33">
+        <v>5416</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>24.69</v>
+      </c>
+      <c r="G33">
+        <v>3.7</v>
+      </c>
+      <c r="H33">
+        <v>51.11</v>
+      </c>
+      <c r="J33" t="s">
+        <v>134</v>
+      </c>
+      <c r="K33" t="s">
+        <v>5</v>
+      </c>
+      <c r="L33">
+        <v>270</v>
+      </c>
+      <c r="M33">
+        <v>27068</v>
+      </c>
+      <c r="N33">
+        <v>4</v>
+      </c>
+      <c r="O33">
+        <v>14.81</v>
+      </c>
+      <c r="P33">
+        <v>1.5</v>
+      </c>
+      <c r="Q33">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>751</v>
+      </c>
+      <c r="D34">
+        <v>75943</v>
+      </c>
+      <c r="E34">
+        <v>18</v>
+      </c>
+      <c r="F34">
+        <v>23.97</v>
+      </c>
+      <c r="G34">
+        <v>2.4</v>
+      </c>
+      <c r="H34">
+        <v>50</v>
+      </c>
+      <c r="J34" t="s">
+        <v>135</v>
+      </c>
+      <c r="K34" t="s">
+        <v>23</v>
+      </c>
+      <c r="L34">
+        <v>68</v>
+      </c>
+      <c r="M34">
+        <v>6510</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>14.71</v>
+      </c>
+      <c r="P34">
+        <v>1.5</v>
+      </c>
+      <c r="Q34">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35">
+        <v>84</v>
+      </c>
+      <c r="D35">
+        <v>8670</v>
+      </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>23.81</v>
+      </c>
+      <c r="G35">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H35">
+        <v>51.11</v>
+      </c>
+      <c r="J35" t="s">
+        <v>136</v>
+      </c>
+      <c r="K35" t="s">
+        <v>33</v>
+      </c>
+      <c r="L35">
+        <v>68</v>
+      </c>
+      <c r="M35">
+        <v>6649</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>14.71</v>
+      </c>
+      <c r="P35">
+        <v>1.5</v>
+      </c>
+      <c r="Q35">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36">
+        <v>89</v>
+      </c>
+      <c r="D36">
+        <v>8233</v>
+      </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>22.47</v>
+      </c>
+      <c r="G36">
+        <v>2.4</v>
+      </c>
+      <c r="H36">
+        <v>51.11</v>
+      </c>
+      <c r="J36" t="s">
+        <v>137</v>
+      </c>
+      <c r="K36" t="s">
+        <v>33</v>
+      </c>
+      <c r="L36">
+        <v>138</v>
+      </c>
+      <c r="M36">
+        <v>10895</v>
+      </c>
+      <c r="N36">
+        <v>2</v>
+      </c>
+      <c r="O36">
+        <v>14.49</v>
+      </c>
+      <c r="P36">
+        <v>1.8</v>
+      </c>
+      <c r="Q36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37">
+        <v>93</v>
+      </c>
+      <c r="D37">
+        <v>6638</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>21.51</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+      <c r="H37">
+        <v>51.11</v>
+      </c>
+      <c r="J37" t="s">
+        <v>138</v>
+      </c>
+      <c r="K37" t="s">
+        <v>26</v>
+      </c>
+      <c r="L37">
+        <v>277</v>
+      </c>
+      <c r="M37">
+        <v>28184</v>
+      </c>
+      <c r="N37">
+        <v>4</v>
+      </c>
+      <c r="O37">
+        <v>14.44</v>
+      </c>
+      <c r="P37">
+        <v>1.4</v>
+      </c>
+      <c r="Q37">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>13</v>
+      </c>
+      <c r="C38">
+        <v>93</v>
+      </c>
+      <c r="D38">
+        <v>12871</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>21.51</v>
+      </c>
+      <c r="G38">
+        <v>1.6</v>
+      </c>
+      <c r="H38">
+        <v>51.11</v>
+      </c>
+      <c r="J38" t="s">
+        <v>139</v>
+      </c>
+      <c r="K38" t="s">
+        <v>13</v>
+      </c>
+      <c r="L38">
+        <v>70</v>
+      </c>
+      <c r="M38">
+        <v>8285</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>14.29</v>
+      </c>
+      <c r="P38">
+        <v>1.2</v>
+      </c>
+      <c r="Q38">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39">
+        <v>196</v>
+      </c>
+      <c r="D39">
+        <v>19525</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39">
+        <v>20.41</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>50</v>
+      </c>
+      <c r="J39" t="s">
+        <v>140</v>
+      </c>
+      <c r="K39" t="s">
+        <v>23</v>
+      </c>
+      <c r="L39">
+        <v>70</v>
+      </c>
+      <c r="M39">
+        <v>6823</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>14.29</v>
+      </c>
+      <c r="P39">
+        <v>1.5</v>
+      </c>
+      <c r="Q39">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C40">
+        <v>109</v>
+      </c>
+      <c r="D40">
+        <v>7562</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="G40">
+        <v>2.6</v>
+      </c>
+      <c r="H40">
+        <v>51.11</v>
+      </c>
+      <c r="J40" t="s">
+        <v>141</v>
+      </c>
+      <c r="K40" t="s">
+        <v>13</v>
+      </c>
+      <c r="L40">
+        <v>71</v>
+      </c>
+      <c r="M40">
+        <v>7600</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>14.08</v>
+      </c>
+      <c r="P40">
+        <v>1.3</v>
+      </c>
+      <c r="Q40">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41">
+        <v>164</v>
+      </c>
+      <c r="D41">
+        <v>15280</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>18.29</v>
+      </c>
+      <c r="G41">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>51.11</v>
+      </c>
+      <c r="J41" t="s">
+        <v>142</v>
+      </c>
+      <c r="K41" t="s">
+        <v>33</v>
+      </c>
+      <c r="L41">
+        <v>361</v>
+      </c>
+      <c r="M41">
+        <v>32564</v>
+      </c>
+      <c r="N41">
+        <v>5</v>
+      </c>
+      <c r="O41">
+        <v>13.85</v>
+      </c>
+      <c r="P41">
+        <v>1.5</v>
+      </c>
+      <c r="Q41">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42">
+        <v>220</v>
+      </c>
+      <c r="D42">
+        <v>24632</v>
+      </c>
+      <c r="E42">
+        <v>4</v>
+      </c>
+      <c r="F42">
+        <v>18.18</v>
+      </c>
+      <c r="G42">
+        <v>1.6</v>
+      </c>
+      <c r="H42">
+        <v>50</v>
+      </c>
+      <c r="J42" t="s">
+        <v>143</v>
+      </c>
+      <c r="K42" t="s">
+        <v>14</v>
+      </c>
+      <c r="L42">
+        <v>73</v>
+      </c>
+      <c r="M42">
+        <v>7411</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+      <c r="O42">
+        <v>13.7</v>
+      </c>
+      <c r="P42">
+        <v>1.3</v>
+      </c>
+      <c r="Q42">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" t="s">
+        <v>13</v>
+      </c>
+      <c r="C43">
+        <v>111</v>
+      </c>
+      <c r="D43">
+        <v>12040</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>18.02</v>
+      </c>
+      <c r="G43">
+        <v>1.7</v>
+      </c>
+      <c r="H43">
+        <v>51.11</v>
+      </c>
+      <c r="J43" t="s">
+        <v>144</v>
+      </c>
+      <c r="K43" t="s">
+        <v>31</v>
+      </c>
+      <c r="L43">
+        <v>305</v>
+      </c>
+      <c r="M43">
+        <v>23751</v>
+      </c>
+      <c r="N43">
+        <v>4</v>
+      </c>
+      <c r="O43">
+        <v>13.11</v>
+      </c>
+      <c r="P43">
+        <v>1.7</v>
+      </c>
+      <c r="Q43">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>114</v>
+      </c>
+      <c r="B44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44">
+        <v>353</v>
+      </c>
+      <c r="D44">
+        <v>24155</v>
+      </c>
+      <c r="E44">
+        <v>6</v>
+      </c>
+      <c r="F44">
+        <v>17</v>
+      </c>
+      <c r="G44">
+        <v>2.5</v>
+      </c>
+      <c r="H44">
+        <v>50</v>
+      </c>
+      <c r="J44" t="s">
+        <v>145</v>
+      </c>
+      <c r="K44" t="s">
+        <v>6</v>
+      </c>
+      <c r="L44">
+        <v>699</v>
+      </c>
+      <c r="M44">
+        <v>80094</v>
+      </c>
+      <c r="N44">
+        <v>9</v>
+      </c>
+      <c r="O44">
+        <v>12.88</v>
+      </c>
+      <c r="P44">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q44">
+        <v>51.25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>115</v>
+      </c>
+      <c r="B45" t="s">
+        <v>31</v>
+      </c>
+      <c r="C45">
+        <v>59</v>
+      </c>
+      <c r="D45">
+        <v>5184</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>16.95</v>
+      </c>
+      <c r="G45">
+        <v>1.9</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="J45" t="s">
+        <v>146</v>
+      </c>
+      <c r="K45" t="s">
+        <v>5</v>
+      </c>
+      <c r="L45">
+        <v>311</v>
+      </c>
+      <c r="M45">
+        <v>32351</v>
+      </c>
+      <c r="N45">
+        <v>4</v>
+      </c>
+      <c r="O45">
+        <v>12.86</v>
+      </c>
+      <c r="P45">
+        <v>1.2</v>
+      </c>
+      <c r="Q45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>116</v>
+      </c>
+      <c r="B46" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46">
+        <v>599</v>
+      </c>
+      <c r="D46">
+        <v>42595</v>
+      </c>
+      <c r="E46">
+        <v>10</v>
+      </c>
+      <c r="F46">
+        <v>16.690000000000001</v>
+      </c>
+      <c r="G46">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="H46">
+        <v>53</v>
+      </c>
+      <c r="J46" t="s">
+        <v>147</v>
+      </c>
+      <c r="K46" t="s">
+        <v>25</v>
+      </c>
+      <c r="L46">
+        <v>78</v>
+      </c>
+      <c r="M46">
+        <v>8931</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>12.82</v>
+      </c>
+      <c r="P46">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q46">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C47">
+        <v>186</v>
+      </c>
+      <c r="D47">
+        <v>15381</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47">
+        <v>16.13</v>
+      </c>
+      <c r="G47">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>50</v>
+      </c>
+      <c r="J47" t="s">
+        <v>148</v>
+      </c>
+      <c r="K47" t="s">
+        <v>5</v>
+      </c>
+      <c r="L47">
+        <v>321</v>
+      </c>
+      <c r="M47">
+        <v>33442</v>
+      </c>
+      <c r="N47">
+        <v>4</v>
+      </c>
+      <c r="O47">
+        <v>12.46</v>
+      </c>
+      <c r="P47">
+        <v>1.2</v>
+      </c>
+      <c r="Q47">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>118</v>
+      </c>
+      <c r="B48" t="s">
+        <v>13</v>
+      </c>
+      <c r="C48">
+        <v>62</v>
+      </c>
+      <c r="D48">
+        <v>6920</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>16.13</v>
+      </c>
+      <c r="G48">
+        <v>1.4</v>
+      </c>
+      <c r="H48">
+        <v>51.11</v>
+      </c>
+      <c r="J48" t="s">
+        <v>149</v>
+      </c>
+      <c r="K48" t="s">
+        <v>18</v>
+      </c>
+      <c r="L48">
+        <v>886</v>
+      </c>
+      <c r="M48">
+        <v>134583</v>
+      </c>
+      <c r="N48">
+        <v>11</v>
+      </c>
+      <c r="O48">
+        <v>12.42</v>
+      </c>
+      <c r="P48">
+        <v>0.8</v>
+      </c>
+      <c r="Q48">
+        <v>53.33</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>119</v>
+      </c>
+      <c r="B49" t="s">
+        <v>17</v>
+      </c>
+      <c r="C49">
+        <v>63</v>
+      </c>
+      <c r="D49">
+        <v>7089</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>15.87</v>
+      </c>
+      <c r="G49">
+        <v>1.4</v>
+      </c>
+      <c r="H49">
+        <v>51.11</v>
+      </c>
+      <c r="J49" t="s">
+        <v>150</v>
+      </c>
+      <c r="K49" t="s">
+        <v>33</v>
+      </c>
+      <c r="L49">
+        <v>82</v>
+      </c>
+      <c r="M49">
+        <v>6694</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>12.2</v>
+      </c>
+      <c r="P49">
+        <v>1.5</v>
+      </c>
+      <c r="Q49">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50">
+        <v>130</v>
+      </c>
+      <c r="D50">
+        <v>12044</v>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+      <c r="F50">
+        <v>15.38</v>
+      </c>
+      <c r="G50">
+        <v>1.7</v>
+      </c>
+      <c r="H50">
+        <v>51.11</v>
+      </c>
+      <c r="J50" t="s">
+        <v>151</v>
+      </c>
+      <c r="K50" t="s">
+        <v>33</v>
+      </c>
+      <c r="L50">
+        <v>412</v>
+      </c>
+      <c r="M50">
+        <v>33361</v>
+      </c>
+      <c r="N50">
+        <v>5</v>
+      </c>
+      <c r="O50">
+        <v>12.14</v>
+      </c>
+      <c r="P50">
+        <v>1.5</v>
+      </c>
+      <c r="Q50">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>121</v>
+      </c>
+      <c r="B51" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51">
+        <v>66</v>
+      </c>
+      <c r="D51">
+        <v>6975</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>15.15</v>
+      </c>
+      <c r="G51">
+        <v>1.4</v>
+      </c>
+      <c r="H51">
+        <v>51.11</v>
+      </c>
+      <c r="J51" t="s">
+        <v>152</v>
+      </c>
+      <c r="K51" t="s">
+        <v>3</v>
+      </c>
+      <c r="L51">
+        <v>171</v>
+      </c>
+      <c r="M51">
+        <v>19254</v>
+      </c>
+      <c r="N51">
+        <v>2</v>
+      </c>
+      <c r="O51">
+        <v>11.7</v>
+      </c>
+      <c r="P51">
+        <v>1</v>
+      </c>
+      <c r="Q51">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>122</v>
+      </c>
+      <c r="B52" t="s">
+        <v>30</v>
+      </c>
+      <c r="C52">
+        <v>138</v>
+      </c>
+      <c r="D52">
+        <v>15318</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>14.49</v>
+      </c>
+      <c r="G52">
+        <v>1.3</v>
+      </c>
+      <c r="H52">
+        <v>51.11</v>
+      </c>
+      <c r="J52" t="s">
+        <v>153</v>
+      </c>
+      <c r="K52" t="s">
+        <v>11</v>
+      </c>
+      <c r="L52">
+        <v>86</v>
+      </c>
+      <c r="M52">
+        <v>9151</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>11.63</v>
+      </c>
+      <c r="P52">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q52">
+        <v>51.11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" t="s">
+        <v>34</v>
+      </c>
+      <c r="C53">
+        <v>71</v>
+      </c>
+      <c r="D53">
+        <v>6239</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>14.08</v>
+      </c>
+      <c r="G53">
+        <v>1.6</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="J53" t="s">
+        <v>154</v>
+      </c>
+      <c r="K53" t="s">
+        <v>33</v>
+      </c>
+      <c r="L53">
+        <v>88</v>
+      </c>
+      <c r="M53">
+        <v>8557</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>11.36</v>
+      </c>
+      <c r="P53">
+        <v>1.2</v>
+      </c>
+      <c r="Q53">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>